<commit_message>
Updated utility tests and associated upload spreadsheet fixtures
Updated all of the dummy spreadsheets to use the data
template. Updated the tests that verify the shape and contents of the
uploaded spreadsheet to use the new upload template. Tests associated
with the event form, and integration tests associated with the data
upload continue to fail.
</commit_message>
<xml_diff>
--- a/fsdviz/tests/xls_files/good_one_record.xlsx
+++ b/fsdviz/tests/xls_files/good_one_record.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COTTRILLAD\1work\LakeTrout\Stocking\GLFSD_Datavis\fsdviz\fsdviz\tests\xls_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33C36E7-6CDE-4E63-B86F-69902A959B9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E6A5E1-5E9F-4BAE-89D1-D4AA1DA72004}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StockingEvents" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>stock_id</t>
   </si>
@@ -109,9 +109,6 @@
     <t>agency</t>
   </si>
   <si>
-    <t>validation</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -149,6 +146,18 @@
   </si>
   <si>
     <t>MNRF</t>
+  </si>
+  <si>
+    <t>hatchery</t>
+  </si>
+  <si>
+    <t>agency_stock_id</t>
+  </si>
+  <si>
+    <t>CFCW</t>
+  </si>
+  <si>
+    <t>X9999</t>
   </si>
 </sst>
 </file>
@@ -488,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,15 +597,18 @@
         <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>30</v>
+        <v>42</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
       <c r="D2">
         <v>2015</v>
@@ -608,7 +620,7 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2">
         <v>42.342241799999996</v>
@@ -620,13 +632,13 @@
         <v>214</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P2">
         <v>18149</v>
@@ -635,13 +647,13 @@
         <v>2014</v>
       </c>
       <c r="R2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S2">
         <v>18</v>
       </c>
       <c r="T2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U2">
         <v>99.5</v>
@@ -662,16 +674,22 @@
         <v>1</v>
       </c>
       <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>42</v>
-      </c>
       <c r="AE2" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>